<commit_message>
Small fix: standardised cost_variable_om
</commit_message>
<xml_diff>
--- a/data/zenodo_ivan/extraction/CHE_ext_biogas.xlsx
+++ b/data/zenodo_ivan/extraction/CHE_ext_biogas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruiziv/switchdrive/ACCURACY/RESTORE/data/zenodo_ivan/extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08EC3D3-3C3B-1A47-B519-51D078AEE150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ACE996-C3F6-3141-948C-9C3A8F4DDFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17500" yWindow="500" windowWidth="20900" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>proven_reserves</t>
   </si>
   <si>
-    <t>cost_variable</t>
-  </si>
-  <si>
     <t>CHE_ext_biogas.xlsx</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>constant_fxe</t>
+  </si>
+  <si>
+    <t>cost_variable_om</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -600,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -662,7 +662,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -677,16 +677,16 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -698,7 +698,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>17</v>
@@ -710,16 +710,16 @@
         <v>5.2841010000000006</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -727,7 +727,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>24</v>
@@ -737,7 +737,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -745,10 +745,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -762,10 +762,10 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -779,10 +779,10 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -796,10 +796,10 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -813,10 +813,10 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -830,10 +830,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
@@ -847,10 +847,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
@@ -864,10 +864,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
@@ -881,10 +881,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -898,10 +898,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -915,10 +915,10 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -932,10 +932,10 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -949,10 +949,10 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -966,10 +966,10 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -983,10 +983,10 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
@@ -1000,10 +1000,10 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -1017,10 +1017,10 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
         <v>22</v>
@@ -1034,10 +1034,10 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
         <v>22</v>
@@ -1051,10 +1051,10 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
@@ -1068,10 +1068,10 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
@@ -1085,10 +1085,10 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -1100,16 +1100,16 @@
         <v>6.1484170000000002</v>
       </c>
       <c r="H30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" t="s">
         <v>29</v>
       </c>
-      <c r="J30" t="s">
-        <v>30</v>
-      </c>
       <c r="K30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -1117,10 +1117,10 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
@@ -1134,10 +1134,10 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
         <v>22</v>
@@ -1151,10 +1151,10 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
         <v>22</v>
@@ -1168,10 +1168,10 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
@@ -1185,10 +1185,10 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D35" t="s">
         <v>22</v>
@@ -1202,10 +1202,10 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
@@ -1219,10 +1219,10 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -1236,10 +1236,10 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
         <v>22</v>
@@ -1253,10 +1253,10 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
         <v>22</v>

</xml_diff>